<commit_message>
Flussi aggiornati al 8 Gennaio 2020
</commit_message>
<xml_diff>
--- a/data/pagopa-intermediari.xlsx
+++ b/data/pagopa-intermediari.xlsx
@@ -91,7 +91,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8599</t>
+          <t>8603</t>
         </is>
       </c>
     </row>
@@ -125,7 +125,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>802</t>
+          <t>809</t>
         </is>
       </c>
     </row>
@@ -142,7 +142,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>585</t>
+          <t>604</t>
         </is>
       </c>
     </row>
@@ -159,7 +159,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>508</t>
         </is>
       </c>
     </row>
@@ -176,7 +176,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>440</t>
+          <t>443</t>
         </is>
       </c>
     </row>
@@ -210,7 +210,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>416</t>
+          <t>418</t>
         </is>
       </c>
     </row>
@@ -227,7 +227,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>376</t>
         </is>
       </c>
     </row>
@@ -244,7 +244,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>351</t>
+          <t>357</t>
         </is>
       </c>
     </row>
@@ -278,7 +278,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>249</t>
         </is>
       </c>
     </row>
@@ -295,7 +295,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>246</t>
         </is>
       </c>
     </row>
@@ -329,7 +329,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>198</t>
+          <t>200</t>
         </is>
       </c>
     </row>
@@ -363,7 +363,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>177</t>
         </is>
       </c>
     </row>
@@ -397,7 +397,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>167</t>
         </is>
       </c>
     </row>
@@ -438,68 +438,68 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Regione Toscana</t>
+          <t>Siscom SPA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>01386030488</t>
+          <t>01778000040</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>115</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Next Step Solution</t>
+          <t>Regione Toscana</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>02554480349</t>
+          <t>01386030488</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>113</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Regione Basilicata</t>
+          <t>Next Step Solution</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>80002950766</t>
+          <t>02554480349</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>111</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Siscom SPA</t>
+          <t>Regione Basilicata</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>01778000040</t>
+          <t>80002950766</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>106</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>80</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>73</t>
         </is>
       </c>
     </row>
@@ -608,102 +608,102 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>NORDCOM</t>
+          <t>Regione Umbria</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>13384100155</t>
+          <t>80000130544</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>57</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Regione Umbria</t>
+          <t>NORDCOM</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>80000130544</t>
+          <t>13384100155</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>56</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Italriscossioni Società Italiana di Fiscalità Locale S.r.l.</t>
+          <t>DCS SOFTWARE E SERVIZI S.R.L.</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06092371001</t>
+          <t>08063140019</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>52</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Bluenext S.r.l.</t>
+          <t>Italriscossioni Società Italiana di Fiscalità Locale S.r.l.</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>04228480408</t>
+          <t>06092371001</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>50</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CINECA consorzio universitario</t>
+          <t>Bluenext S.r.l.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>00317740371</t>
+          <t>04228480408</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>46</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DCS SOFTWARE E SERVIZI S.R.L.</t>
+          <t>CINECA consorzio universitario</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>08063140019</t>
+          <t>00317740371</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>44</t>
         </is>
       </c>
     </row>
@@ -720,7 +720,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>43</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>35</t>
         </is>
       </c>
     </row>
@@ -788,7 +788,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>34</t>
         </is>
       </c>
     </row>
@@ -829,29 +829,29 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Citta' Metropolitana di Roma Capitale</t>
+          <t>Comune di Palermo</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>80034390585</t>
+          <t>80016350821</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>24</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Nexi SpA</t>
+          <t>Citta' Metropolitana di Roma Capitale</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>13212880150</t>
+          <t>80034390585</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -863,29 +863,29 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ANDREANI TRIBUTI srl</t>
+          <t>Nexi SpA</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>01412920439</t>
+          <t>13212880150</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Regione Lazio</t>
+          <t>ANDREANI TRIBUTI srl</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>80143490581</t>
+          <t>01412920439</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -897,29 +897,29 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Comune di Palermo</t>
+          <t>Regione Lazio</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>80016350821</t>
+          <t>80143490581</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Si.Form Consulting srl</t>
+          <t>Servizi Locali SpA</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>03943960827</t>
+          <t>03170580751</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -931,12 +931,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Servizi Locali SpA</t>
+          <t>Si.Form Consulting srl</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>03170580751</t>
+          <t>03943960827</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -948,12 +948,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Aric Agenzia Regionale di Informatica e Committenza</t>
+          <t>Crédit Agricole Group Solutions Società Consortile per azioni</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>91022630676</t>
+          <t>02771790348</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -965,63 +965,63 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Crédit Agricole Group Solutions Società Consortile per azioni</t>
+          <t>Aric Agenzia Regionale di Informatica e Committenza</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>02771790348</t>
+          <t>91022630676</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>UBI Banca</t>
+          <t>Comune di Catania</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>03053920165</t>
+          <t>00137020871</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Comune di Catania</t>
+          <t>UBI Banca</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>00137020871</t>
+          <t>03053920165</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ARCA Servizi s.r.l</t>
+          <t>Be Smart s.r.l.</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>09106071005</t>
+          <t>05817461006</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1033,12 +1033,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Be Smart s.r.l.</t>
+          <t>ARCA Servizi s.r.l</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>05817461006</t>
+          <t>09106071005</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1060,19 +1060,19 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ARGO SOFTWARE SRL</t>
+          <t>Phoenix IT Solutions S.r.L</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>00838520880</t>
+          <t>07623321218</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1084,12 +1084,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Phoenix IT Solutions S.r.L</t>
+          <t>CityPoste Payment Digital S.r.l.</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>07623321218</t>
+          <t>02003750672</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1101,12 +1101,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>CityPoste Payment Digital S.r.l.</t>
+          <t>ARGO SOFTWARE SRL</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>02003750672</t>
+          <t>00838520880</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1118,12 +1118,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>e-SED Società Cooperativa</t>
+          <t>Linea Comune Spa</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>02695640421</t>
+          <t>05591950489</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1135,12 +1135,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Linea Comune Spa</t>
+          <t>e-SED Società Cooperativa</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>05591950489</t>
+          <t>02695640421</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1169,12 +1169,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>KOINE' SRL</t>
+          <t>Softline srl</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>01934790971</t>
+          <t>12299030150</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1186,12 +1186,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ICCREA Banca SpA</t>
+          <t>KOINE' SRL</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>04774801007</t>
+          <t>01934790971</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1203,29 +1203,29 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>I.C.A. - Imposte Comunali Affini – s.r.l.</t>
+          <t>ICCREA Banca SpA</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>02478610583</t>
+          <t>04774801007</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Agenzia Italiana del Farmaco - AIFA</t>
+          <t>BANCA MONTE DEI PASCHI DI SIENA</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>97345810580</t>
+          <t>00884060526</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1237,12 +1237,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Banco BPM Società per Azioni</t>
+          <t>Società Almaviva S.p.A.</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>09722490969</t>
+          <t>08450891000</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1254,12 +1254,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Ministero dello Sviluppo Economico</t>
+          <t>Banca Nazionale del Lavoro S.p.A.</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>80230390587</t>
+          <t>09339391006</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1271,12 +1271,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Noviservice srl</t>
+          <t>Banco BPM Società per Azioni</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>02789990922</t>
+          <t>09722490969</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1288,12 +1288,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Softline srl</t>
+          <t>Engineering Ingegneria Informatica SpA</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>12299030150</t>
+          <t>00967720285</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1305,12 +1305,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MegASP S.r.l.</t>
+          <t>Noviservice srl</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>09898030151</t>
+          <t>02789990922</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1322,12 +1322,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Banca Nazionale del Lavoro S.p.A.</t>
+          <t>MegASP S.r.l.</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>09339391006</t>
+          <t>09898030151</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1339,12 +1339,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Engineering Ingegneria Informatica SpA</t>
+          <t>I.C.A. - Imposte Comunali Affini – s.r.l.</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>00967720285</t>
+          <t>02478610583</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1356,12 +1356,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>BANCA MONTE DEI PASCHI DI SIENA</t>
+          <t>Agenzia Italiana del Farmaco - AIFA</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>00884060526</t>
+          <t>97345810580</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1373,12 +1373,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>San Marco SPA</t>
+          <t>Ministero dello Sviluppo Economico</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>04142440728</t>
+          <t>80230390587</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Società Almaviva S.p.A.</t>
+          <t>San Marco SPA</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>08450891000</t>
+          <t>04142440728</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">

</xml_diff>

<commit_message>
Flussi aggiornati al 16 Gennaio 2020
</commit_message>
<xml_diff>
--- a/data/pagopa-intermediari.xlsx
+++ b/data/pagopa-intermediari.xlsx
@@ -108,7 +108,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1080</t>
+          <t>1083</t>
         </is>
       </c>
     </row>
@@ -142,7 +142,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>604</t>
+          <t>608</t>
         </is>
       </c>
     </row>
@@ -159,7 +159,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>508</t>
+          <t>511</t>
         </is>
       </c>
     </row>
@@ -193,7 +193,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>424</t>
+          <t>429</t>
         </is>
       </c>
     </row>
@@ -210,7 +210,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>420</t>
         </is>
       </c>
     </row>
@@ -244,7 +244,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>357</t>
+          <t>362</t>
         </is>
       </c>
     </row>
@@ -278,7 +278,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>252</t>
         </is>
       </c>
     </row>
@@ -295,7 +295,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>246</t>
+          <t>249</t>
         </is>
       </c>
     </row>
@@ -312,7 +312,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>227</t>
         </is>
       </c>
     </row>
@@ -329,7 +329,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>203</t>
         </is>
       </c>
     </row>
@@ -363,7 +363,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>177</t>
+          <t>181</t>
         </is>
       </c>
     </row>
@@ -380,7 +380,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>170</t>
         </is>
       </c>
     </row>
@@ -397,7 +397,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>170</t>
         </is>
       </c>
     </row>
@@ -431,7 +431,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>127</t>
         </is>
       </c>
     </row>
@@ -448,7 +448,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>122</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>82</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>69</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>61</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>51</t>
         </is>
       </c>
     </row>
@@ -788,7 +788,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>35</t>
         </is>
       </c>
     </row>
@@ -822,7 +822,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>30</t>
         </is>
       </c>
     </row>
@@ -846,12 +846,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Citta' Metropolitana di Roma Capitale</t>
+          <t>Nexi SpA</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>80034390585</t>
+          <t>13212880150</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -863,12 +863,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Nexi SpA</t>
+          <t>Citta' Metropolitana di Roma Capitale</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>13212880150</t>
+          <t>80034390585</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -914,12 +914,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Servizi Locali SpA</t>
+          <t>Si.Form Consulting srl</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>03170580751</t>
+          <t>03943960827</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -931,12 +931,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Si.Form Consulting srl</t>
+          <t>Servizi Locali SpA</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>03943960827</t>
+          <t>03170580751</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -982,12 +982,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Comune di Catania</t>
+          <t>UBI Banca</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>00137020871</t>
+          <t>03053920165</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -999,12 +999,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>UBI Banca</t>
+          <t>Comune di Catania</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>03053920165</t>
+          <t>00137020871</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1016,29 +1016,29 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Be Smart s.r.l.</t>
+          <t>ARCA Servizi s.r.l</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>05817461006</t>
+          <t>09106071005</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>ARCA Servizi s.r.l</t>
+          <t>Be Smart s.r.l.</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>09106071005</t>
+          <t>05817461006</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1067,29 +1067,29 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Phoenix IT Solutions S.r.L</t>
+          <t>ARGO SOFTWARE SRL</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>07623321218</t>
+          <t>00838520880</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>CityPoste Payment Digital S.r.l.</t>
+          <t>Phoenix IT Solutions S.r.L</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>02003750672</t>
+          <t>07623321218</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1101,12 +1101,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>ARGO SOFTWARE SRL</t>
+          <t>CityPoste Payment Digital S.r.l.</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>00838520880</t>
+          <t>02003750672</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1118,12 +1118,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Linea Comune Spa</t>
+          <t>ISWEB S.p.A.</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>05591950489</t>
+          <t>01722270665</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1152,12 +1152,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ISWEB S.p.A.</t>
+          <t>Linea Comune Spa</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>01722270665</t>
+          <t>05591950489</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1169,12 +1169,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Softline srl</t>
+          <t>KOINE' SRL</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>12299030150</t>
+          <t>01934790971</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1186,12 +1186,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>KOINE' SRL</t>
+          <t>Softline srl</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>01934790971</t>
+          <t>12299030150</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1220,12 +1220,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>BANCA MONTE DEI PASCHI DI SIENA</t>
+          <t>San Marco SPA</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>00884060526</t>
+          <t>04142440728</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1237,12 +1237,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Società Almaviva S.p.A.</t>
+          <t>BANCA MONTE DEI PASCHI DI SIENA</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>08450891000</t>
+          <t>00884060526</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1254,12 +1254,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Banca Nazionale del Lavoro S.p.A.</t>
+          <t>Società Almaviva S.p.A.</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09339391006</t>
+          <t>08450891000</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1271,12 +1271,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Banco BPM Società per Azioni</t>
+          <t>Engineering Ingegneria Informatica SpA</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>09722490969</t>
+          <t>00967720285</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1288,12 +1288,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Engineering Ingegneria Informatica SpA</t>
+          <t>Banco BPM Società per Azioni</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>00967720285</t>
+          <t>09722490969</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1305,12 +1305,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Noviservice srl</t>
+          <t>Ministero dello Sviluppo Economico</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>02789990922</t>
+          <t>80230390587</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1322,12 +1322,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>MegASP S.r.l.</t>
+          <t>Agenzia Italiana del Farmaco - AIFA</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>09898030151</t>
+          <t>97345810580</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1339,12 +1339,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>I.C.A. - Imposte Comunali Affini – s.r.l.</t>
+          <t>Noviservice srl</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>02478610583</t>
+          <t>02789990922</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1356,12 +1356,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Agenzia Italiana del Farmaco - AIFA</t>
+          <t>Banca Nazionale del Lavoro S.p.A.</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>97345810580</t>
+          <t>09339391006</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1373,12 +1373,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Ministero dello Sviluppo Economico</t>
+          <t>MegASP S.r.l.</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>80230390587</t>
+          <t>09898030151</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>San Marco SPA</t>
+          <t>I.C.A. - Imposte Comunali Affini – s.r.l.</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>04142440728</t>
+          <t>02478610583</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">

</xml_diff>

<commit_message>
Update flussi del 29 Gennaio 2020
</commit_message>
<xml_diff>
--- a/data/pagopa-intermediari.xlsx
+++ b/data/pagopa-intermediari.xlsx
@@ -81,7 +81,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ministero dell'Istruzione, dell'Universita' e della Ricerca</t>
+          <t>Ministero dell'Istruzione, Ministero dell'Universita' e della Ricerca</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -108,7 +108,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1083</t>
+          <t>1084</t>
         </is>
       </c>
     </row>
@@ -125,7 +125,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>809</t>
+          <t>812</t>
         </is>
       </c>
     </row>
@@ -142,7 +142,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>608</t>
+          <t>633</t>
         </is>
       </c>
     </row>
@@ -159,7 +159,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>511</t>
+          <t>513</t>
         </is>
       </c>
     </row>
@@ -176,7 +176,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>443</t>
+          <t>452</t>
         </is>
       </c>
     </row>
@@ -193,7 +193,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>429</t>
+          <t>430</t>
         </is>
       </c>
     </row>
@@ -210,7 +210,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>421</t>
         </is>
       </c>
     </row>
@@ -227,7 +227,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>376</t>
+          <t>380</t>
         </is>
       </c>
     </row>
@@ -244,7 +244,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>362</t>
+          <t>369</t>
         </is>
       </c>
     </row>
@@ -278,7 +278,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>255</t>
         </is>
       </c>
     </row>
@@ -295,7 +295,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>254</t>
         </is>
       </c>
     </row>
@@ -312,7 +312,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>227</t>
+          <t>238</t>
         </is>
       </c>
     </row>
@@ -329,41 +329,41 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>203</t>
+          <t>205</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Alto Adige Riscossioni Spa</t>
+          <t>Regione Marche</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>02805390214</t>
+          <t>80008630420</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>183</t>
+          <t>184</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Regione Marche</t>
+          <t>Alto Adige Riscossioni Spa</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>80008630420</t>
+          <t>02805390214</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>183</t>
         </is>
       </c>
     </row>
@@ -380,7 +380,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>174</t>
         </is>
       </c>
     </row>
@@ -397,7 +397,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>173</t>
         </is>
       </c>
     </row>
@@ -421,68 +421,68 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Regione Puglia</t>
+          <t>Siscom SPA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>80017210727</t>
+          <t>01778000040</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>128</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Siscom SPA</t>
+          <t>Regione Puglia</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>01778000040</t>
+          <t>80017210727</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>127</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Regione Toscana</t>
+          <t>Next Step Solution</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>01386030488</t>
+          <t>02554480349</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>118</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Next Step Solution</t>
+          <t>Regione Toscana</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>02554480349</t>
+          <t>01386030488</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>115</t>
         </is>
       </c>
     </row>
@@ -533,7 +533,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>87</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>84</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>81</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>75</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>63</t>
         </is>
       </c>
     </row>
@@ -652,7 +652,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>53</t>
         </is>
       </c>
     </row>
@@ -754,7 +754,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>39</t>
         </is>
       </c>
     </row>
@@ -805,7 +805,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>34</t>
         </is>
       </c>
     </row>
@@ -822,7 +822,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>31</t>
         </is>
       </c>
     </row>
@@ -948,12 +948,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Crédit Agricole Group Solutions Società Consortile per azioni</t>
+          <t>Aric Agenzia Regionale di Informatica e Committenza</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>02771790348</t>
+          <t>91022630676</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -965,12 +965,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Aric Agenzia Regionale di Informatica e Committenza</t>
+          <t>Crédit Agricole Group Solutions Società Consortile per azioni</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>91022630676</t>
+          <t>02771790348</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -992,7 +992,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
     </row>
@@ -1033,12 +1033,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Be Smart s.r.l.</t>
+          <t>Argentea S.r.l.</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>05817461006</t>
+          <t>02260390220</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1050,12 +1050,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Argentea S.r.l.</t>
+          <t>Noviservice srl</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>02260390220</t>
+          <t>02789990922</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1067,34 +1067,34 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>ARGO SOFTWARE SRL</t>
+          <t>Be Smart s.r.l.</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>00838520880</t>
+          <t>05817461006</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Phoenix IT Solutions S.r.L</t>
+          <t>ARGO SOFTWARE SRL</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>07623321218</t>
+          <t>00838520880</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1118,17 +1118,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>ISWEB S.p.A.</t>
+          <t>Phoenix IT Solutions S.r.L</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>01722270665</t>
+          <t>07623321218</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1152,12 +1152,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Linea Comune Spa</t>
+          <t>ISWEB S.p.A.</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>05591950489</t>
+          <t>01722270665</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1169,29 +1169,29 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>KOINE' SRL</t>
+          <t>Linea Comune Spa</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>01934790971</t>
+          <t>05591950489</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Softline srl</t>
+          <t>KOINE' SRL</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>12299030150</t>
+          <t>01934790971</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1220,46 +1220,46 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>San Marco SPA</t>
+          <t>Regione Calabria</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>04142440728</t>
+          <t>02205340793</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>BANCA MONTE DEI PASCHI DI SIENA</t>
+          <t>Softline srl</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>00884060526</t>
+          <t>12299030150</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Società Almaviva S.p.A.</t>
+          <t>San Marco SPA</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>08450891000</t>
+          <t>04142440728</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1288,12 +1288,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Banco BPM Società per Azioni</t>
+          <t>Società Almaviva S.p.A.</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>09722490969</t>
+          <t>08450891000</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1305,12 +1305,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Ministero dello Sviluppo Economico</t>
+          <t>Agenzia Italiana del Farmaco - AIFA</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>80230390587</t>
+          <t>97345810580</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1322,12 +1322,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Agenzia Italiana del Farmaco - AIFA</t>
+          <t>I.C.A. - Imposte Comunali Affini – s.r.l.</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>97345810580</t>
+          <t>02478610583</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1339,12 +1339,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Noviservice srl</t>
+          <t>BANCA MONTE DEI PASCHI DI SIENA</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>02789990922</t>
+          <t>00884060526</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1356,12 +1356,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Banca Nazionale del Lavoro S.p.A.</t>
+          <t>Open Software S.r.l.</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>09339391006</t>
+          <t>02810000279</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1373,12 +1373,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>MegASP S.r.l.</t>
+          <t>Banco BPM Società per Azioni</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>09898030151</t>
+          <t>09722490969</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1390,15 +1390,66 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>I.C.A. - Imposte Comunali Affini – s.r.l.</t>
+          <t>WAN S.r.l.</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>02478610583</t>
+          <t>03805290040</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Banca Nazionale del Lavoro S.p.A.</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>09339391006</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Ministero dello Sviluppo Economico</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>80230390587</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>MegASP S.r.l.</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>09898030151</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
         <is>
           <t>1</t>
         </is>

</xml_diff>